<commit_message>
Rimligare antal aktiva bilar
</commit_message>
<xml_diff>
--- a/em.xlsx
+++ b/em.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G86"/>
+  <dimension ref="A1:G84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,42 +473,38 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Individ 20</t>
+          <t>Individ 6</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
           <t>('Eftermiddag', '13-15')</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>cat</t>
-        </is>
-      </c>
+      <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
-          <t>BergsbyvÃ¤gen 19</t>
+          <t>Rudagatan 18</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>64.72253627756791</t>
+          <t>64.72822387894983</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>21.081495540234208</t>
+          <t>21.066092511399347</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Individ 21</t>
+          <t>Individ 15</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -521,29 +517,29 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>&gt;18</t>
+          <t>smoker,dog,&gt;18</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Nybyggargatan 12</t>
+          <t>Getargatan 13</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>64.72279765876095</t>
+          <t>64.72515988986189</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>21.096477997904646</t>
+          <t>21.081590156187488</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Individ 24</t>
+          <t>Individ 18</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -554,31 +550,35 @@
           <t>('Eftermiddag', '13-15')</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>license,&gt;18</t>
+        </is>
+      </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Roddargatan 12</t>
+          <t>OmvÃ¤gen 11</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>64.71749269547423</t>
+          <t>64.722700477568</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>21.09246261139871</t>
+          <t>21.076038097904636</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Individ 28</t>
+          <t>Individ 20</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -587,33 +587,33 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>license,cat</t>
+          <t>cat</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Lillgatan 7A</t>
+          <t>BergsbyvÃ¤gen 19</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>64.71565457756343</t>
+          <t>64.72253627756791</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>21.0969892402338</t>
+          <t>21.081495540234208</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Individ 29</t>
+          <t>Individ 21</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -622,161 +622,169 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>license</t>
+          <t>&gt;18</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Roddargatan 29</t>
+          <t>Nybyggargatan 12</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>64.7158097128137</t>
+          <t>64.72279765876095</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>21.098717311398616</t>
+          <t>21.096477997904646</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Individ 41</t>
+          <t>Individ 24</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
           <t>('Eftermiddag', '13-15')</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>license</t>
-        </is>
-      </c>
+      <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr">
         <is>
-          <t>SkelleftehamnsvÃ¤gen 113</t>
+          <t>Roddargatan 12</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>64.7145646253258</t>
+          <t>64.71749269547423</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>21.16073439790411</t>
+          <t>21.09246261139871</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Individ 44</t>
+          <t>Individ 28</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
           <t>('Eftermiddag', '13-15')</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr"/>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>license,cat</t>
+        </is>
+      </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>VÃ¤nskapsgatan 4</t>
+          <t>Lillgatan 7A</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>64.71183961148486</t>
+          <t>64.71565457756343</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>21.17002340955187</t>
+          <t>21.0969892402338</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Individ 59</t>
+          <t>Individ 29</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
           <t>('Eftermiddag', '13-15')</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr"/>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>license</t>
+        </is>
+      </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Lotsens grÃ¤nd 5</t>
+          <t>Roddargatan 29</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>64.69594034903153</t>
+          <t>64.7158097128137</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>21.190897069067788</t>
+          <t>21.098717311398616</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Individ 62</t>
+          <t>Individ 41</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
           <t>('Eftermiddag', '13-15')</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr"/>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>license</t>
+        </is>
+      </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>VÃ¥gens grÃ¤nd 2</t>
+          <t>SkelleftehamnsvÃ¤gen 113</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>64.69386766364026</t>
+          <t>64.7145646253258</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>21.195669282562054</t>
+          <t>21.16073439790411</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Individ 69</t>
+          <t>Individ 44</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -786,24 +794,24 @@
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr">
         <is>
-          <t>BokgrÃ¤nd 7</t>
+          <t>VÃ¤nskapsgatan 4</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>64.71491237756301</t>
+          <t>64.71183961148486</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>21.158029382563345</t>
+          <t>21.17002340955187</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Individ 1</t>
+          <t>Individ 59</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -811,104 +819,96 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>('Middag', '15-17')</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>license,dog</t>
-        </is>
-      </c>
+          <t>('Eftermiddag', '13-15')</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Rudagatan 51</t>
+          <t>Lotsens grÃ¤nd 5</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>64.73076905004987</t>
+          <t>64.69594034903153</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>21.062869127380175</t>
+          <t>21.190897069067788</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Individ 2</t>
+          <t>Individ 62</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>('Middag', '15-17')</t>
+          <t>('Eftermiddag', '13-15')</t>
         </is>
       </c>
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Rudagatan 41</t>
+          <t>VÃ¥gens grÃ¤nd 2</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>64.73109609499264</t>
+          <t>64.69386766364026</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>21.065514656793624</t>
+          <t>21.195669282562054</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Individ 3</t>
+          <t>Individ 69</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>('Middag', '15-17')</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>smoker</t>
-        </is>
-      </c>
+          <t>('Eftermiddag', '13-15')</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Rudagatan 69</t>
+          <t>BokgrÃ¤nd 7</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>64.72923223634149</t>
+          <t>64.71491237756301</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>21.063728215696155</t>
+          <t>21.158029382563345</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Individ 5</t>
+          <t>Individ 1</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -917,33 +917,33 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>&gt;18</t>
+          <t>license,dog</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Rudagatan 13</t>
+          <t>Rudagatan 51</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>64.7290092981411</t>
+          <t>64.73076905004987</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>21.067118011399394</t>
+          <t>21.062869127380175</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Individ 6</t>
+          <t>Individ 2</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -953,59 +953,63 @@
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Rudagatan 18</t>
+          <t>Rudagatan 41</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>64.72822387894983</t>
+          <t>64.73109609499264</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>21.066092511399347</t>
+          <t>21.065514656793624</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Individ 6</t>
+          <t>Individ 3</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
           <t>('Middag', '15-17')</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr"/>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>smoker</t>
+        </is>
+      </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Rudagatan 18</t>
+          <t>Rudagatan 69</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>64.72822387894983</t>
+          <t>64.72923223634149</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>21.066092511399347</t>
+          <t>21.063728215696155</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Individ 13</t>
+          <t>Individ 5</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -1014,33 +1018,33 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>license,&gt;18</t>
+          <t>&gt;18</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>DiktorpsvÃ¤gen 14</t>
+          <t>Rudagatan 13</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>64.72742231880282</t>
+          <t>64.7290092981411</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>21.07853091139931</t>
+          <t>21.067118011399394</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Individ 16</t>
+          <t>Individ 6</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -1050,24 +1054,24 @@
       <c r="D19" t="inlineStr"/>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Johansgatan 27</t>
+          <t>Rudagatan 18</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>64.72402676388035</t>
+          <t>64.72822387894983</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>21.080091374591447</t>
+          <t>21.066092511399347</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Individ 18</t>
+          <t>Individ 6</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -1078,66 +1082,66 @@
           <t>('Middag', '15-17')</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>license,&gt;18</t>
-        </is>
-      </c>
+      <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr">
         <is>
-          <t>OmvÃ¤gen 11</t>
+          <t>Rudagatan 18</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>64.722700477568</t>
+          <t>64.72822387894983</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>21.076038097904636</t>
+          <t>21.066092511399347</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Individ 19</t>
+          <t>Individ 13</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
           <t>('Middag', '15-17')</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr"/>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>license,&gt;18</t>
+        </is>
+      </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Holmgatan 22</t>
+          <t>DiktorpsvÃ¤gen 14</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>64.72178804029595</t>
+          <t>64.72742231880282</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>21.078316140234115</t>
+          <t>21.07853091139931</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Individ 24</t>
+          <t>Individ 16</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -1147,28 +1151,28 @@
       <c r="D22" t="inlineStr"/>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Roddargatan 12</t>
+          <t>Johansgatan 27</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>64.71749269547423</t>
+          <t>64.72402676388035</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>21.09246261139871</t>
+          <t>21.080091374591447</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Individ 40</t>
+          <t>Individ 18</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -1177,231 +1181,231 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>license</t>
+          <t>license,&gt;18</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Karagangatan 7</t>
+          <t>OmvÃ¤gen 11</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>64.71669937756415</t>
+          <t>64.722700477568</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>21.16159071139863</t>
+          <t>21.076038097904636</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Individ 40</t>
+          <t>Individ 19</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
           <t>('Middag', '15-17')</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>license</t>
-        </is>
-      </c>
+      <c r="D24" t="inlineStr"/>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Karagangatan 7</t>
+          <t>Holmgatan 22</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>64.71669937756415</t>
+          <t>64.72178804029595</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>21.16159071139863</t>
+          <t>21.078316140234115</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Individ 41</t>
+          <t>Individ 24</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
           <t>('Middag', '15-17')</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>license</t>
-        </is>
-      </c>
+      <c r="D25" t="inlineStr"/>
       <c r="E25" t="inlineStr">
         <is>
-          <t>SkelleftehamnsvÃ¤gen 113</t>
+          <t>Roddargatan 12</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>64.7145646253258</t>
+          <t>64.71749269547423</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>21.16073439790411</t>
+          <t>21.09246261139871</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Individ 51</t>
+          <t>Individ 40</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
           <t>('Middag', '15-17')</t>
         </is>
       </c>
-      <c r="D26" t="inlineStr"/>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>license</t>
+        </is>
+      </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>SkyttevÃ¤gen 3</t>
+          <t>Karagangatan 7</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>64.70942679485121</t>
+          <t>64.71669937756415</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>21.17345478256298</t>
+          <t>21.16159071139863</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Individ 53</t>
+          <t>Individ 40</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
           <t>('Middag', '15-17')</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr"/>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>license</t>
+        </is>
+      </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Redargatan 11</t>
+          <t>Karagangatan 7</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>64.70674759364812</t>
+          <t>64.71669937756415</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>21.18053518256285</t>
+          <t>21.16159071139863</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Individ 54</t>
+          <t>Individ 41</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
           <t>('Middag', '15-17')</t>
         </is>
       </c>
-      <c r="D28" t="inlineStr"/>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>license</t>
+        </is>
+      </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Redargatan 14</t>
+          <t>SkelleftehamnsvÃ¤gen 113</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>64.70605796158435</t>
+          <t>64.7145646253258</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>21.180770669068398</t>
+          <t>21.16073439790411</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Individ 57</t>
+          <t>Individ 51</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
           <t>('Middag', '15-17')</t>
         </is>
       </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>license</t>
-        </is>
-      </c>
+      <c r="D29" t="inlineStr"/>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Ã–rlogsgatan 28</t>
+          <t>SkyttevÃ¤gen 3</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>64.70277797755517</t>
+          <t>64.70942679485121</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>21.18806254023302</t>
+          <t>21.17345478256298</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Individ 62</t>
+          <t>Individ 53</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -1411,28 +1415,28 @@
       <c r="D30" t="inlineStr"/>
       <c r="E30" t="inlineStr">
         <is>
-          <t>VÃ¥gens grÃ¤nd 2</t>
+          <t>Redargatan 11</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>64.69386766364026</t>
+          <t>64.70674759364812</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>21.195669282562054</t>
+          <t>21.18053518256285</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Individ 65</t>
+          <t>Individ 54</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
@@ -1442,59 +1446,63 @@
       <c r="D31" t="inlineStr"/>
       <c r="E31" t="inlineStr">
         <is>
-          <t>HARRBÃ„CKSSAND 152</t>
+          <t>Redargatan 14</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>64.72430178226789</t>
+          <t>64.70605796158435</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>21.227400740234213</t>
+          <t>21.180770669068398</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Individ 67</t>
+          <t>Individ 57</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
           <t>('Middag', '15-17')</t>
         </is>
       </c>
-      <c r="D32" t="inlineStr"/>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>license</t>
+        </is>
+      </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Styrmansgatan 9</t>
+          <t>Ã–rlogsgatan 28</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>64.70799259606436</t>
+          <t>64.70277797755517</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>21.178082469068517</t>
+          <t>21.18806254023302</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Individ 69</t>
+          <t>Individ 62</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -1504,160 +1512,152 @@
       <c r="D33" t="inlineStr"/>
       <c r="E33" t="inlineStr">
         <is>
-          <t>BokgrÃ¤nd 7</t>
+          <t>VÃ¥gens grÃ¤nd 2</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>64.71491237756301</t>
+          <t>64.69386766364026</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>21.158029382563345</t>
+          <t>21.195669282562054</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Individ 2</t>
+          <t>Individ 65</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>('Tidig kväll', '17-19')</t>
+          <t>('Middag', '15-17')</t>
         </is>
       </c>
       <c r="D34" t="inlineStr"/>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Rudagatan 41</t>
+          <t>HARRBÃ„CKSSAND 152</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>64.73109609499264</t>
+          <t>64.72430178226789</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>21.065514656793624</t>
+          <t>21.227400740234213</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Individ 6</t>
+          <t>Individ 67</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>('Tidig kväll', '17-19')</t>
+          <t>('Middag', '15-17')</t>
         </is>
       </c>
       <c r="D35" t="inlineStr"/>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Rudagatan 18</t>
+          <t>Styrmansgatan 9</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>64.72822387894983</t>
+          <t>64.70799259606436</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>21.066092511399347</t>
+          <t>21.178082469068517</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Individ 14</t>
+          <t>Individ 69</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>('Tidig kväll', '17-19')</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>dog</t>
-        </is>
-      </c>
+          <t>('Middag', '15-17')</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr"/>
       <c r="E36" t="inlineStr">
         <is>
-          <t>TrÃ¶skargatan 12</t>
+          <t>BokgrÃ¤nd 7</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>64.72569273438936</t>
+          <t>64.71491237756301</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>21.08245052745085</t>
+          <t>21.158029382563345</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Individ 15</t>
+          <t>Individ 2</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
           <t>('Tidig kväll', '17-19')</t>
         </is>
       </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>smoker,dog,&gt;18</t>
-        </is>
-      </c>
+      <c r="D37" t="inlineStr"/>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Getargatan 13</t>
+          <t>Rudagatan 41</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>64.72515988986189</t>
+          <t>64.73109609499264</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>21.081590156187488</t>
+          <t>21.065514656793624</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Individ 16</t>
+          <t>Individ 6</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1667,24 +1667,24 @@
       <c r="D38" t="inlineStr"/>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Johansgatan 27</t>
+          <t>Rudagatan 18</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>64.72402676388035</t>
+          <t>64.72822387894983</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>21.080091374591447</t>
+          <t>21.066092511399347</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Individ 28</t>
+          <t>Individ 14</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1697,64 +1697,68 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>license,cat</t>
+          <t>dog</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Lillgatan 7A</t>
+          <t>TrÃ¶skargatan 12</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>64.71565457756343</t>
+          <t>64.72569273438936</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>21.0969892402338</t>
+          <t>21.08245052745085</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Individ 36</t>
+          <t>Individ 15</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
           <t>('Tidig kväll', '17-19')</t>
         </is>
       </c>
-      <c r="D40" t="inlineStr"/>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>smoker,dog,&gt;18</t>
+        </is>
+      </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>SkelleftehamnsvÃ¤gen 80</t>
+          <t>Getargatan 13</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>64.7163138775638</t>
+          <t>64.72515988986189</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>21.15327989790421</t>
+          <t>21.081590156187488</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Individ 53</t>
+          <t>Individ 16</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -1764,24 +1768,24 @@
       <c r="D41" t="inlineStr"/>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Redargatan 11</t>
+          <t>Johansgatan 27</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>64.70674759364812</t>
+          <t>64.72402676388035</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>21.18053518256285</t>
+          <t>21.080091374591447</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Individ 54</t>
+          <t>Individ 28</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -1792,27 +1796,31 @@
           <t>('Tidig kväll', '17-19')</t>
         </is>
       </c>
-      <c r="D42" t="inlineStr"/>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>license,cat</t>
+        </is>
+      </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Redargatan 14</t>
+          <t>Lillgatan 7A</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>64.70605796158435</t>
+          <t>64.71565457756343</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>21.180770669068398</t>
+          <t>21.0969892402338</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Individ 57</t>
+          <t>Individ 36</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -1823,31 +1831,27 @@
           <t>('Tidig kväll', '17-19')</t>
         </is>
       </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>license</t>
-        </is>
-      </c>
+      <c r="D43" t="inlineStr"/>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Ã–rlogsgatan 28</t>
+          <t>SkelleftehamnsvÃ¤gen 80</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>64.70277797755517</t>
+          <t>64.7163138775638</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>21.18806254023302</t>
+          <t>21.15327989790421</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Individ 60</t>
+          <t>Individ 53</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -1858,31 +1862,27 @@
           <t>('Tidig kväll', '17-19')</t>
         </is>
       </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>license</t>
-        </is>
-      </c>
+      <c r="D44" t="inlineStr"/>
       <c r="E44" t="inlineStr">
         <is>
-          <t>AlderholmsvÃ¤gen 30</t>
+          <t>Redargatan 11</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>64.6949387916413</t>
+          <t>64.70674759364812</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>21.189652311397285</t>
+          <t>21.18053518256285</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Individ 61</t>
+          <t>Individ 54</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -1893,93 +1893,97 @@
           <t>('Tidig kväll', '17-19')</t>
         </is>
       </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>license</t>
-        </is>
-      </c>
+      <c r="D45" t="inlineStr"/>
       <c r="E45" t="inlineStr">
         <is>
-          <t>SkelleftehamnsvÃ¤gen 205</t>
+          <t>Redargatan 14</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>64.6956845633339</t>
+          <t>64.70605796158435</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>21.198373724891763</t>
+          <t>21.180770669068398</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Individ 62</t>
+          <t>Individ 57</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
           <t>('Tidig kväll', '17-19')</t>
         </is>
       </c>
-      <c r="D46" t="inlineStr"/>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>license</t>
+        </is>
+      </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>VÃ¥gens grÃ¤nd 2</t>
+          <t>Ã–rlogsgatan 28</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>64.69386766364026</t>
+          <t>64.70277797755517</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>21.195669282562054</t>
+          <t>21.18806254023302</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Individ 65</t>
+          <t>Individ 60</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
           <t>('Tidig kväll', '17-19')</t>
         </is>
       </c>
-      <c r="D47" t="inlineStr"/>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>license</t>
+        </is>
+      </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>HARRBÃ„CKSSAND 152</t>
+          <t>AlderholmsvÃ¤gen 30</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>64.72430178226789</t>
+          <t>64.6949387916413</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>21.227400740234213</t>
+          <t>21.189652311397285</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Individ 67</t>
+          <t>Individ 61</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -1990,31 +1994,35 @@
           <t>('Tidig kväll', '17-19')</t>
         </is>
       </c>
-      <c r="D48" t="inlineStr"/>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>license</t>
+        </is>
+      </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Styrmansgatan 9</t>
+          <t>SkelleftehamnsvÃ¤gen 205</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>64.70799259606436</t>
+          <t>64.6956845633339</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>21.178082469068517</t>
+          <t>21.198373724891763</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Individ 69</t>
+          <t>Individ 62</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
@@ -2024,152 +2032,152 @@
       <c r="D49" t="inlineStr"/>
       <c r="E49" t="inlineStr">
         <is>
-          <t>BokgrÃ¤nd 7</t>
+          <t>VÃ¥gens grÃ¤nd 2</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>64.71491237756301</t>
+          <t>64.69386766364026</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>21.158029382563345</t>
+          <t>21.195669282562054</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Individ 1</t>
+          <t>Individ 65</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>('Sen kväll', '19-21')</t>
-        </is>
-      </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t>license,dog</t>
-        </is>
-      </c>
+          <t>('Tidig kväll', '17-19')</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr"/>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Rudagatan 51</t>
+          <t>HARRBÃ„CKSSAND 152</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>64.73076905004987</t>
+          <t>64.72430178226789</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>21.062869127380175</t>
+          <t>21.227400740234213</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Individ 2</t>
+          <t>Individ 67</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>('Sen kväll', '19-21')</t>
+          <t>('Tidig kväll', '17-19')</t>
         </is>
       </c>
       <c r="D51" t="inlineStr"/>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Rudagatan 41</t>
+          <t>Styrmansgatan 9</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>64.73109609499264</t>
+          <t>64.70799259606436</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>21.065514656793624</t>
+          <t>21.178082469068517</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Individ 6</t>
+          <t>Individ 69</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>('Sen kväll', '19-21')</t>
+          <t>('Tidig kväll', '17-19')</t>
         </is>
       </c>
       <c r="D52" t="inlineStr"/>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Rudagatan 18</t>
+          <t>BokgrÃ¤nd 7</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>64.72822387894983</t>
+          <t>64.71491237756301</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>21.066092511399347</t>
+          <t>21.158029382563345</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Individ 6</t>
+          <t>Individ 1</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
           <t>('Sen kväll', '19-21')</t>
         </is>
       </c>
-      <c r="D53" t="inlineStr"/>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>license,dog</t>
+        </is>
+      </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Rudagatan 18</t>
+          <t>Rudagatan 51</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>64.72822387894983</t>
+          <t>64.73076905004987</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>21.066092511399347</t>
+          <t>21.062869127380175</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Individ 8</t>
+          <t>Individ 2</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -2183,133 +2191,121 @@
       <c r="D54" t="inlineStr"/>
       <c r="E54" t="inlineStr">
         <is>
-          <t>FalmyrvÃ¤gen 58</t>
+          <t>Rudagatan 41</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>64.72731282540025</t>
+          <t>64.73109609499264</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>21.07195383043295</t>
+          <t>21.065514656793624</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Individ 13</t>
+          <t>Individ 6</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
           <t>('Sen kväll', '19-21')</t>
         </is>
       </c>
-      <c r="D55" t="inlineStr">
-        <is>
-          <t>license,&gt;18</t>
-        </is>
-      </c>
+      <c r="D55" t="inlineStr"/>
       <c r="E55" t="inlineStr">
         <is>
-          <t>DiktorpsvÃ¤gen 14</t>
+          <t>Rudagatan 18</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>64.72742231880282</t>
+          <t>64.72822387894983</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>21.07853091139931</t>
+          <t>21.066092511399347</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Individ 14</t>
+          <t>Individ 6</t>
         </is>
       </c>
       <c r="B56" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
           <t>('Sen kväll', '19-21')</t>
         </is>
       </c>
-      <c r="D56" t="inlineStr">
-        <is>
-          <t>dog</t>
-        </is>
-      </c>
+      <c r="D56" t="inlineStr"/>
       <c r="E56" t="inlineStr">
         <is>
-          <t>TrÃ¶skargatan 12</t>
+          <t>Rudagatan 18</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>64.72569273438936</t>
+          <t>64.72822387894983</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>21.08245052745085</t>
+          <t>21.066092511399347</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Individ 15</t>
+          <t>Individ 8</t>
         </is>
       </c>
       <c r="B57" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
           <t>('Sen kväll', '19-21')</t>
         </is>
       </c>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>smoker,dog,&gt;18</t>
-        </is>
-      </c>
+      <c r="D57" t="inlineStr"/>
       <c r="E57" t="inlineStr">
         <is>
-          <t>Getargatan 13</t>
+          <t>FalmyrvÃ¤gen 58</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>64.72515988986189</t>
+          <t>64.72731282540025</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>21.081590156187488</t>
+          <t>21.07195383043295</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Individ 18</t>
+          <t>Individ 13</t>
         </is>
       </c>
       <c r="B58" t="n">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C58" t="inlineStr">
         <is>
@@ -2323,55 +2319,59 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>OmvÃ¤gen 11</t>
+          <t>DiktorpsvÃ¤gen 14</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>64.722700477568</t>
+          <t>64.72742231880282</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>21.076038097904636</t>
+          <t>21.07853091139931</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Individ 19</t>
+          <t>Individ 14</t>
         </is>
       </c>
       <c r="B59" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
           <t>('Sen kväll', '19-21')</t>
         </is>
       </c>
-      <c r="D59" t="inlineStr"/>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>dog</t>
+        </is>
+      </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>Holmgatan 22</t>
+          <t>TrÃ¶skargatan 12</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>64.72178804029595</t>
+          <t>64.72569273438936</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>21.078316140234115</t>
+          <t>21.08245052745085</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Individ 20</t>
+          <t>Individ 15</t>
         </is>
       </c>
       <c r="B60" t="n">
@@ -2384,33 +2384,33 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>cat</t>
+          <t>smoker,dog,&gt;18</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>BergsbyvÃ¤gen 19</t>
+          <t>Getargatan 13</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>64.72253627756791</t>
+          <t>64.72515988986189</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>21.081495540234208</t>
+          <t>21.081590156187488</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Individ 21</t>
+          <t>Individ 18</t>
         </is>
       </c>
       <c r="B61" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
@@ -2419,95 +2419,95 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>&gt;18</t>
+          <t>license,&gt;18</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>Nybyggargatan 12</t>
+          <t>OmvÃ¤gen 11</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>64.72279765876095</t>
+          <t>64.722700477568</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>21.096477997904646</t>
+          <t>21.076038097904636</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Individ 22</t>
+          <t>Individ 19</t>
         </is>
       </c>
       <c r="B62" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
           <t>('Sen kväll', '19-21')</t>
         </is>
       </c>
-      <c r="D62" t="inlineStr">
-        <is>
-          <t>dog</t>
-        </is>
-      </c>
+      <c r="D62" t="inlineStr"/>
       <c r="E62" t="inlineStr">
         <is>
-          <t>Nybyggargatan 13</t>
+          <t>Holmgatan 22</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>64.7221138654314</t>
+          <t>64.72178804029595</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>21.096186911398974</t>
+          <t>21.078316140234115</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Individ 23</t>
+          <t>Individ 20</t>
         </is>
       </c>
       <c r="B63" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
           <t>('Sen kväll', '19-21')</t>
         </is>
       </c>
-      <c r="D63" t="inlineStr"/>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>cat</t>
+        </is>
+      </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>Nybyggargatan 6B</t>
+          <t>BergsbyvÃ¤gen 19</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>64.71991329588566</t>
+          <t>64.72253627756791</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>21.094155711398862</t>
+          <t>21.081495540234208</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Individ 24</t>
+          <t>Individ 21</t>
         </is>
       </c>
       <c r="B64" t="n">
@@ -2518,27 +2518,31 @@
           <t>('Sen kväll', '19-21')</t>
         </is>
       </c>
-      <c r="D64" t="inlineStr"/>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>&gt;18</t>
+        </is>
+      </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>Roddargatan 12</t>
+          <t>Nybyggargatan 12</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>64.71749269547423</t>
+          <t>64.72279765876095</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>21.09246261139871</t>
+          <t>21.096477997904646</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Individ 26</t>
+          <t>Individ 22</t>
         </is>
       </c>
       <c r="B65" t="n">
@@ -2549,136 +2553,128 @@
           <t>('Sen kväll', '19-21')</t>
         </is>
       </c>
-      <c r="D65" t="inlineStr"/>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>dog</t>
+        </is>
+      </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>Roddargatan 17</t>
+          <t>Nybyggargatan 13</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>64.7169136063257</t>
+          <t>64.7221138654314</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>21.09606822673948</t>
+          <t>21.096186911398974</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Individ 27</t>
+          <t>Individ 23</t>
         </is>
       </c>
       <c r="B66" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
           <t>('Sen kväll', '19-21')</t>
         </is>
       </c>
-      <c r="D66" t="inlineStr">
-        <is>
-          <t>smoker,&gt;18</t>
-        </is>
-      </c>
+      <c r="D66" t="inlineStr"/>
       <c r="E66" t="inlineStr">
         <is>
-          <t>Lillgatan 4</t>
+          <t>Nybyggargatan 6B</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>64.71611465988815</t>
+          <t>64.71991329588566</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>21.09484154023385</t>
+          <t>21.094155711398862</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Individ 39</t>
+          <t>Individ 24</t>
         </is>
       </c>
       <c r="B67" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
           <t>('Sen kväll', '19-21')</t>
         </is>
       </c>
-      <c r="D67" t="inlineStr">
-        <is>
-          <t>smoker</t>
-        </is>
-      </c>
+      <c r="D67" t="inlineStr"/>
       <c r="E67" t="inlineStr">
         <is>
-          <t>MÃ¥bÃ¤rsgatan 9</t>
+          <t>Roddargatan 12</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>64.71710435972129</t>
+          <t>64.71749269547423</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>21.156185624893038</t>
+          <t>21.09246261139871</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Individ 40</t>
+          <t>Individ 26</t>
         </is>
       </c>
       <c r="B68" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
           <t>('Sen kväll', '19-21')</t>
         </is>
       </c>
-      <c r="D68" t="inlineStr">
-        <is>
-          <t>license</t>
-        </is>
-      </c>
+      <c r="D68" t="inlineStr"/>
       <c r="E68" t="inlineStr">
         <is>
-          <t>Karagangatan 7</t>
+          <t>Roddargatan 17</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>64.71669937756415</t>
+          <t>64.7169136063257</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>21.16159071139863</t>
+          <t>21.09606822673948</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Individ 40</t>
+          <t>Individ 27</t>
         </is>
       </c>
       <c r="B69" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
@@ -2687,33 +2683,33 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>license</t>
+          <t>smoker,&gt;18</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>Karagangatan 7</t>
+          <t>Lillgatan 4</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>64.71669937756415</t>
+          <t>64.71611465988815</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>21.16159071139863</t>
+          <t>21.09484154023385</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Individ 41</t>
+          <t>Individ 39</t>
         </is>
       </c>
       <c r="B70" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
@@ -2722,126 +2718,138 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>license</t>
+          <t>smoker</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>SkelleftehamnsvÃ¤gen 113</t>
+          <t>MÃ¥bÃ¤rsgatan 9</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>64.7145646253258</t>
+          <t>64.71710435972129</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>21.16073439790411</t>
+          <t>21.156185624893038</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Individ 47</t>
+          <t>Individ 40</t>
         </is>
       </c>
       <c r="B71" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
           <t>('Sen kväll', '19-21')</t>
         </is>
       </c>
-      <c r="D71" t="inlineStr"/>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>license</t>
+        </is>
+      </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>SandgÃ¤rdsvÃ¤gen 33</t>
+          <t>Karagangatan 7</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>64.71030057755999</t>
+          <t>64.71669937756415</t>
         </is>
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>21.18197034023344</t>
+          <t>21.16159071139863</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Individ 50</t>
+          <t>Individ 40</t>
         </is>
       </c>
       <c r="B72" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
           <t>('Sen kväll', '19-21')</t>
         </is>
       </c>
-      <c r="D72" t="inlineStr"/>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>license</t>
+        </is>
+      </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>BrÃ¶drahemsgatan 16</t>
+          <t>Karagangatan 7</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>64.71090737756037</t>
+          <t>64.71669937756415</t>
         </is>
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>21.17480491139828</t>
+          <t>21.16159071139863</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Individ 51</t>
+          <t>Individ 41</t>
         </is>
       </c>
       <c r="B73" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
           <t>('Sen kväll', '19-21')</t>
         </is>
       </c>
-      <c r="D73" t="inlineStr"/>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>license</t>
+        </is>
+      </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>SkyttevÃ¤gen 3</t>
+          <t>SkelleftehamnsvÃ¤gen 113</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>64.70942679485121</t>
+          <t>64.7145646253258</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>21.17345478256298</t>
+          <t>21.16073439790411</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Individ 59</t>
+          <t>Individ 47</t>
         </is>
       </c>
       <c r="B74" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C74" t="inlineStr">
         <is>
@@ -2851,28 +2859,28 @@
       <c r="D74" t="inlineStr"/>
       <c r="E74" t="inlineStr">
         <is>
-          <t>Lotsens grÃ¤nd 5</t>
+          <t>SandgÃ¤rdsvÃ¤gen 33</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>64.69594034903153</t>
+          <t>64.71030057755999</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>21.190897069067788</t>
+          <t>21.18197034023344</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Individ 63</t>
+          <t>Individ 50</t>
         </is>
       </c>
       <c r="B75" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
@@ -2882,28 +2890,28 @@
       <c r="D75" t="inlineStr"/>
       <c r="E75" t="inlineStr">
         <is>
-          <t>SÃ¶dra Sillskatan 510</t>
+          <t>BrÃ¶drahemsgatan 16</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>64.72975809755901</t>
+          <t>64.71090737756037</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>21.220638097905063</t>
+          <t>21.17480491139828</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Individ 70</t>
+          <t>Individ 51</t>
         </is>
       </c>
       <c r="B76" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
@@ -2913,339 +2921,285 @@
       <c r="D76" t="inlineStr"/>
       <c r="E76" t="inlineStr">
         <is>
-          <t>Hagtornsgatan 39</t>
+          <t>SkyttevÃ¤gen 3</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>64.719327050046</t>
+          <t>64.70942679485121</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>21.15099431139883</t>
+          <t>21.17345478256298</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Individ 7</t>
+          <t>Individ 59</t>
         </is>
       </c>
       <c r="B77" t="n">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>('Förmiddag', '9-11')</t>
-        </is>
-      </c>
-      <c r="D77" t="inlineStr">
-        <is>
-          <t>man</t>
-        </is>
-      </c>
+          <t>('Sen kväll', '19-21')</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr"/>
       <c r="E77" t="inlineStr">
         <is>
-          <t>FodergrÃ¤nd 14</t>
+          <t>Lotsens grÃ¤nd 5</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>64.72773447936372</t>
+          <t>64.69594034903153</t>
         </is>
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>21.072368011399337</t>
+          <t>21.190897069067788</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Individ 15</t>
+          <t>Individ 63</t>
         </is>
       </c>
       <c r="B78" t="n">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>('Förmiddag', '9-11')</t>
-        </is>
-      </c>
-      <c r="D78" t="inlineStr">
-        <is>
-          <t>smoker,dog,&gt;18</t>
-        </is>
-      </c>
+          <t>('Sen kväll', '19-21')</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr"/>
       <c r="E78" t="inlineStr">
         <is>
-          <t>Getargatan 13</t>
+          <t>SÃ¶dra Sillskatan 510</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>64.72515988986189</t>
+          <t>64.72975809755901</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>21.081590156187488</t>
+          <t>21.220638097905063</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Individ 16</t>
+          <t>Individ 70</t>
         </is>
       </c>
       <c r="B79" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>('Förmiddag', '9-11')</t>
+          <t>('Sen kväll', '19-21')</t>
         </is>
       </c>
       <c r="D79" t="inlineStr"/>
       <c r="E79" t="inlineStr">
         <is>
-          <t>Johansgatan 27</t>
+          <t>Hagtornsgatan 39</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>64.72402676388035</t>
+          <t>64.719327050046</t>
         </is>
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>21.080091374591447</t>
+          <t>21.15099431139883</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Individ 24</t>
+          <t>Individ 1</t>
         </is>
       </c>
       <c r="B80" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
           <t>('Förmiddag', '9-11')</t>
         </is>
       </c>
-      <c r="D80" t="inlineStr"/>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>license,dog,woman</t>
+        </is>
+      </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>Roddargatan 12</t>
+          <t>Rudagatan 51</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>64.71749269547423</t>
+          <t>64.73076905004987</t>
         </is>
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>21.09246261139871</t>
+          <t>21.062869127380175</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Individ 54</t>
+          <t>Individ 28</t>
         </is>
       </c>
       <c r="B81" t="n">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
           <t>('Förmiddag', '9-11')</t>
         </is>
       </c>
-      <c r="D81" t="inlineStr"/>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>license,cat</t>
+        </is>
+      </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>Redargatan 14</t>
+          <t>Lillgatan 7A</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>64.70605796158435</t>
+          <t>64.71565457756343</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>21.180770669068398</t>
+          <t>21.0969892402338</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Individ 67</t>
+          <t>Individ 29</t>
         </is>
       </c>
       <c r="B82" t="n">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C82" t="inlineStr">
         <is>
           <t>('Förmiddag', '9-11')</t>
         </is>
       </c>
-      <c r="D82" t="inlineStr"/>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>license</t>
+        </is>
+      </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>Styrmansgatan 9</t>
+          <t>Roddargatan 29</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>64.70799259606436</t>
+          <t>64.7158097128137</t>
         </is>
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>21.178082469068517</t>
+          <t>21.098717311398616</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Individ 69</t>
+          <t>Individ 37</t>
         </is>
       </c>
       <c r="B83" t="n">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>('Förmiddag', '9-11')</t>
+          <t>('Eftermiddag', '13-15')</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>woman</t>
+          <t>license</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>BokgrÃ¤nd 7</t>
+          <t>MÃ¥bÃ¤rsgatan 12</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>64.71491237756301</t>
+          <t>64.71651135982128</t>
         </is>
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>21.158029382563345</t>
+          <t>21.15559144023381</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Individ 25</t>
+          <t>Individ 38</t>
         </is>
       </c>
       <c r="B84" t="n">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
           <t>('Eftermiddag', '13-15')</t>
         </is>
       </c>
-      <c r="D84" t="inlineStr"/>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>license</t>
+        </is>
+      </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>Holmgatan 68</t>
+          <t>Karagangatan 30</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>64.7173241596842</t>
+          <t>64.71678347084324</t>
         </is>
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>21.094878711398668</t>
-        </is>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="inlineStr">
-        <is>
-          <t>Individ 35</t>
-        </is>
-      </c>
-      <c r="B85" t="n">
-        <v>60</v>
-      </c>
-      <c r="C85" t="inlineStr">
-        <is>
-          <t>('Eftermiddag', '13-15')</t>
-        </is>
-      </c>
-      <c r="D85" t="inlineStr"/>
-      <c r="E85" t="inlineStr">
-        <is>
-          <t>StapelvÃ¤gen 48B</t>
-        </is>
-      </c>
-      <c r="F85" t="inlineStr">
-        <is>
-          <t>64.71609775989108</t>
-        </is>
-      </c>
-      <c r="G85" t="inlineStr">
-        <is>
-          <t>21.151176282563405</t>
-        </is>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="inlineStr">
-        <is>
-          <t>Individ 42</t>
-        </is>
-      </c>
-      <c r="B86" t="n">
-        <v>30</v>
-      </c>
-      <c r="C86" t="inlineStr">
-        <is>
-          <t>('Eftermiddag', '13-15')</t>
-        </is>
-      </c>
-      <c r="D86" t="inlineStr"/>
-      <c r="E86" t="inlineStr">
-        <is>
-          <t>MekanvÃ¤gen 47</t>
-        </is>
-      </c>
-      <c r="F86" t="inlineStr">
-        <is>
-          <t>64.71201517568417</t>
-        </is>
-      </c>
-      <c r="G86" t="inlineStr">
-        <is>
-          <t>21.155399840233578</t>
+          <t>21.15778882489306</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Funkar nu för fm och em schema
</commit_message>
<xml_diff>
--- a/em.xlsx
+++ b/em.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G84"/>
+  <dimension ref="A1:G66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,178 +473,174 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Individ 6</t>
+          <t>Individ 1</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>('Eftermiddag', '13-15')</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr"/>
+          <t>('Middag', '15-17')</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>license,dog</t>
+        </is>
+      </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Rudagatan 18</t>
+          <t>Rudagatan 51</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>64.72822387894983</t>
+          <t>64.73076905004987</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>21.066092511399347</t>
+          <t>21.062869127380175</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Individ 15</t>
+          <t>Individ 2</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>('Eftermiddag', '13-15')</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>smoker,dog,&gt;18</t>
-        </is>
-      </c>
+          <t>('Middag', '15-17')</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Getargatan 13</t>
+          <t>Rudagatan 41</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>64.72515988986189</t>
+          <t>64.73109609499264</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>21.081590156187488</t>
+          <t>21.065514656793624</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Individ 18</t>
+          <t>Individ 3</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>('Eftermiddag', '13-15')</t>
+          <t>('Middag', '15-17')</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>license,&gt;18</t>
+          <t>smoker</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>OmvÃ¤gen 11</t>
+          <t>Rudagatan 69</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>64.722700477568</t>
+          <t>64.72923223634149</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>21.076038097904636</t>
+          <t>21.063728215696155</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Individ 20</t>
+          <t>Individ 5</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>('Eftermiddag', '13-15')</t>
+          <t>('Middag', '15-17')</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>cat</t>
+          <t>&gt;18</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>BergsbyvÃ¤gen 19</t>
+          <t>Rudagatan 13</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>64.72253627756791</t>
+          <t>64.7290092981411</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>21.081495540234208</t>
+          <t>21.067118011399394</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Individ 21</t>
+          <t>Individ 6</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>('Eftermiddag', '13-15')</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>&gt;18</t>
-        </is>
-      </c>
+          <t>('Middag', '15-17')</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Nybyggargatan 12</t>
+          <t>Rudagatan 18</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>64.72279765876095</t>
+          <t>64.72822387894983</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>21.096477997904646</t>
+          <t>21.066092511399347</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Individ 24</t>
+          <t>Individ 6</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -652,259 +648,263 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>('Eftermiddag', '13-15')</t>
+          <t>('Middag', '15-17')</t>
         </is>
       </c>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Roddargatan 12</t>
+          <t>Rudagatan 18</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>64.71749269547423</t>
+          <t>64.72822387894983</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>21.09246261139871</t>
+          <t>21.066092511399347</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Individ 28</t>
+          <t>Individ 13</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>('Eftermiddag', '13-15')</t>
+          <t>('Middag', '15-17')</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>license,cat</t>
+          <t>license,&gt;18</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Lillgatan 7A</t>
+          <t>DiktorpsvÃ¤gen 14</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>64.71565457756343</t>
+          <t>64.72742231880282</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>21.0969892402338</t>
+          <t>21.07853091139931</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Individ 29</t>
+          <t>Individ 16</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>('Eftermiddag', '13-15')</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>license</t>
-        </is>
-      </c>
+          <t>('Middag', '15-17')</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Roddargatan 29</t>
+          <t>Johansgatan 27</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>64.7158097128137</t>
+          <t>64.72402676388035</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>21.098717311398616</t>
+          <t>21.080091374591447</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Individ 41</t>
+          <t>Individ 18</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>('Eftermiddag', '13-15')</t>
+          <t>('Middag', '15-17')</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>license</t>
+          <t>license,&gt;18</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>SkelleftehamnsvÃ¤gen 113</t>
+          <t>OmvÃ¤gen 11</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>64.7145646253258</t>
+          <t>64.722700477568</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>21.16073439790411</t>
+          <t>21.076038097904636</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Individ 44</t>
+          <t>Individ 19</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>('Eftermiddag', '13-15')</t>
+          <t>('Middag', '15-17')</t>
         </is>
       </c>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr">
         <is>
-          <t>VÃ¤nskapsgatan 4</t>
+          <t>Holmgatan 22</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>64.71183961148486</t>
+          <t>64.72178804029595</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>21.17002340955187</t>
+          <t>21.078316140234115</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Individ 59</t>
+          <t>Individ 24</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>('Eftermiddag', '13-15')</t>
+          <t>('Middag', '15-17')</t>
         </is>
       </c>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Lotsens grÃ¤nd 5</t>
+          <t>Roddargatan 12</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>64.69594034903153</t>
+          <t>64.71749269547423</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>21.190897069067788</t>
+          <t>21.09246261139871</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Individ 62</t>
+          <t>Individ 40</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>('Eftermiddag', '13-15')</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr"/>
+          <t>('Middag', '15-17')</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>license</t>
+        </is>
+      </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>VÃ¥gens grÃ¤nd 2</t>
+          <t>Karagangatan 7</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>64.69386766364026</t>
+          <t>64.71669937756415</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>21.195669282562054</t>
+          <t>21.16159071139863</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Individ 69</t>
+          <t>Individ 40</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>('Eftermiddag', '13-15')</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr"/>
+          <t>('Middag', '15-17')</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>license</t>
+        </is>
+      </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>BokgrÃ¤nd 7</t>
+          <t>Karagangatan 7</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>64.71491237756301</t>
+          <t>64.71669937756415</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>21.158029382563345</t>
+          <t>21.16159071139863</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Individ 1</t>
+          <t>Individ 41</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -917,29 +917,29 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>license,dog</t>
+          <t>license</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Rudagatan 51</t>
+          <t>SkelleftehamnsvÃ¤gen 113</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>64.73076905004987</t>
+          <t>64.7145646253258</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>21.062869127380175</t>
+          <t>21.16073439790411</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Individ 2</t>
+          <t>Individ 51</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -953,59 +953,55 @@
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Rudagatan 41</t>
+          <t>SkyttevÃ¤gen 3</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>64.73109609499264</t>
+          <t>64.70942679485121</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>21.065514656793624</t>
+          <t>21.17345478256298</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Individ 3</t>
+          <t>Individ 53</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
           <t>('Middag', '15-17')</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>smoker</t>
-        </is>
-      </c>
+      <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Rudagatan 69</t>
+          <t>Redargatan 11</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>64.72923223634149</t>
+          <t>64.70674759364812</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>21.063728215696155</t>
+          <t>21.18053518256285</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Individ 5</t>
+          <t>Individ 54</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -1016,31 +1012,27 @@
           <t>('Middag', '15-17')</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>&gt;18</t>
-        </is>
-      </c>
+      <c r="D18" t="inlineStr"/>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Rudagatan 13</t>
+          <t>Redargatan 14</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>64.7290092981411</t>
+          <t>64.70605796158435</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>21.067118011399394</t>
+          <t>21.180770669068398</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Individ 6</t>
+          <t>Individ 57</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -1051,31 +1043,35 @@
           <t>('Middag', '15-17')</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr"/>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>license</t>
+        </is>
+      </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Rudagatan 18</t>
+          <t>Ã–rlogsgatan 28</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>64.72822387894983</t>
+          <t>64.70277797755517</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>21.066092511399347</t>
+          <t>21.18806254023302</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Individ 6</t>
+          <t>Individ 62</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -1085,59 +1081,55 @@
       <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Rudagatan 18</t>
+          <t>VÃ¥gens grÃ¤nd 2</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>64.72822387894983</t>
+          <t>64.69386766364026</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>21.066092511399347</t>
+          <t>21.195669282562054</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Individ 13</t>
+          <t>Individ 65</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
           <t>('Middag', '15-17')</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>license,&gt;18</t>
-        </is>
-      </c>
+      <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr">
         <is>
-          <t>DiktorpsvÃ¤gen 14</t>
+          <t>HARRBÃ„CKSSAND 152</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>64.72742231880282</t>
+          <t>64.72430178226789</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>21.07853091139931</t>
+          <t>21.227400740234213</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Individ 16</t>
+          <t>Individ 67</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -1151,59 +1143,55 @@
       <c r="D22" t="inlineStr"/>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Johansgatan 27</t>
+          <t>Styrmansgatan 9</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>64.72402676388035</t>
+          <t>64.70799259606436</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>21.080091374591447</t>
+          <t>21.178082469068517</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Individ 18</t>
+          <t>Individ 69</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
           <t>('Middag', '15-17')</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>license,&gt;18</t>
-        </is>
-      </c>
+      <c r="D23" t="inlineStr"/>
       <c r="E23" t="inlineStr">
         <is>
-          <t>OmvÃ¤gen 11</t>
+          <t>BokgrÃ¤nd 7</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>64.722700477568</t>
+          <t>64.71491237756301</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>21.076038097904636</t>
+          <t>21.158029382563345</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Individ 19</t>
+          <t>Individ 2</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -1211,30 +1199,30 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>('Middag', '15-17')</t>
+          <t>('Tidig kväll', '17-19')</t>
         </is>
       </c>
       <c r="D24" t="inlineStr"/>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Holmgatan 22</t>
+          <t>Rudagatan 41</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>64.72178804029595</t>
+          <t>64.73109609499264</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>21.078316140234115</t>
+          <t>21.065514656793624</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Individ 24</t>
+          <t>Individ 6</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -1242,294 +1230,294 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>('Middag', '15-17')</t>
+          <t>('Tidig kväll', '17-19')</t>
         </is>
       </c>
       <c r="D25" t="inlineStr"/>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Roddargatan 12</t>
+          <t>Rudagatan 18</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>64.71749269547423</t>
+          <t>64.72822387894983</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>21.09246261139871</t>
+          <t>21.066092511399347</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Individ 40</t>
+          <t>Individ 14</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>('Middag', '15-17')</t>
+          <t>('Tidig kväll', '17-19')</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>license</t>
+          <t>dog</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Karagangatan 7</t>
+          <t>TrÃ¶skargatan 12</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>64.71669937756415</t>
+          <t>64.72569273438936</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>21.16159071139863</t>
+          <t>21.08245052745085</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Individ 40</t>
+          <t>Individ 15</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>('Middag', '15-17')</t>
+          <t>('Tidig kväll', '17-19')</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>license</t>
+          <t>smoker,dog,&gt;18</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Karagangatan 7</t>
+          <t>Getargatan 13</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>64.71669937756415</t>
+          <t>64.72515988986189</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>21.16159071139863</t>
+          <t>21.081590156187488</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Individ 41</t>
+          <t>Individ 16</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>('Middag', '15-17')</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>license</t>
-        </is>
-      </c>
+          <t>('Tidig kväll', '17-19')</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr"/>
       <c r="E28" t="inlineStr">
         <is>
-          <t>SkelleftehamnsvÃ¤gen 113</t>
+          <t>Johansgatan 27</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>64.7145646253258</t>
+          <t>64.72402676388035</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>21.16073439790411</t>
+          <t>21.080091374591447</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Individ 51</t>
+          <t>Individ 28</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>('Middag', '15-17')</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr"/>
+          <t>('Tidig kväll', '17-19')</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>license,cat</t>
+        </is>
+      </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>SkyttevÃ¤gen 3</t>
+          <t>Lillgatan 7A</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>64.70942679485121</t>
+          <t>64.71565457756343</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>21.17345478256298</t>
+          <t>21.0969892402338</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Individ 53</t>
+          <t>Individ 36</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>('Middag', '15-17')</t>
+          <t>('Tidig kväll', '17-19')</t>
         </is>
       </c>
       <c r="D30" t="inlineStr"/>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Redargatan 11</t>
+          <t>SkelleftehamnsvÃ¤gen 80</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>64.70674759364812</t>
+          <t>64.7163138775638</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>21.18053518256285</t>
+          <t>21.15327989790421</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Individ 54</t>
+          <t>Individ 53</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>('Middag', '15-17')</t>
+          <t>('Tidig kväll', '17-19')</t>
         </is>
       </c>
       <c r="D31" t="inlineStr"/>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Redargatan 14</t>
+          <t>Redargatan 11</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>64.70605796158435</t>
+          <t>64.70674759364812</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>21.180770669068398</t>
+          <t>21.18053518256285</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Individ 57</t>
+          <t>Individ 54</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>('Middag', '15-17')</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>license</t>
-        </is>
-      </c>
+          <t>('Tidig kväll', '17-19')</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr"/>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Ã–rlogsgatan 28</t>
+          <t>Redargatan 14</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>64.70277797755517</t>
+          <t>64.70605796158435</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>21.18806254023302</t>
+          <t>21.180770669068398</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Individ 62</t>
+          <t>Individ 57</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>('Middag', '15-17')</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr"/>
+          <t>('Tidig kväll', '17-19')</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>license</t>
+        </is>
+      </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>VÃ¥gens grÃ¤nd 2</t>
+          <t>Ã–rlogsgatan 28</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>64.69386766364026</t>
+          <t>64.70277797755517</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>21.195669282562054</t>
+          <t>21.18806254023302</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Individ 65</t>
+          <t>Individ 60</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -1537,30 +1525,34 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>('Middag', '15-17')</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr"/>
+          <t>('Tidig kväll', '17-19')</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>license</t>
+        </is>
+      </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>HARRBÃ„CKSSAND 152</t>
+          <t>AlderholmsvÃ¤gen 30</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>64.72430178226789</t>
+          <t>64.6949387916413</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>21.227400740234213</t>
+          <t>21.189652311397285</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Individ 67</t>
+          <t>Individ 61</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -1568,65 +1560,69 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>('Middag', '15-17')</t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr"/>
+          <t>('Tidig kväll', '17-19')</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>license</t>
+        </is>
+      </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Styrmansgatan 9</t>
+          <t>SkelleftehamnsvÃ¤gen 205</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>64.70799259606436</t>
+          <t>64.6956845633339</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>21.178082469068517</t>
+          <t>21.198373724891763</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Individ 69</t>
+          <t>Individ 62</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>('Middag', '15-17')</t>
+          <t>('Tidig kväll', '17-19')</t>
         </is>
       </c>
       <c r="D36" t="inlineStr"/>
       <c r="E36" t="inlineStr">
         <is>
-          <t>BokgrÃ¤nd 7</t>
+          <t>VÃ¥gens grÃ¤nd 2</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>64.71491237756301</t>
+          <t>64.69386766364026</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>21.158029382563345</t>
+          <t>21.195669282562054</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Individ 2</t>
+          <t>Individ 65</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -1636,28 +1632,28 @@
       <c r="D37" t="inlineStr"/>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Rudagatan 41</t>
+          <t>HARRBÃ„CKSSAND 152</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>64.73109609499264</t>
+          <t>64.72430178226789</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>21.065514656793624</t>
+          <t>21.227400740234213</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Individ 6</t>
+          <t>Individ 67</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1667,160 +1663,152 @@
       <c r="D38" t="inlineStr"/>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Rudagatan 18</t>
+          <t>Styrmansgatan 9</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>64.72822387894983</t>
+          <t>64.70799259606436</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>21.066092511399347</t>
+          <t>21.178082469068517</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Individ 14</t>
+          <t>Individ 69</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
           <t>('Tidig kväll', '17-19')</t>
         </is>
       </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>dog</t>
-        </is>
-      </c>
+      <c r="D39" t="inlineStr"/>
       <c r="E39" t="inlineStr">
         <is>
-          <t>TrÃ¶skargatan 12</t>
+          <t>BokgrÃ¤nd 7</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>64.72569273438936</t>
+          <t>64.71491237756301</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>21.08245052745085</t>
+          <t>21.158029382563345</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Individ 15</t>
+          <t>Individ 1</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>('Tidig kväll', '17-19')</t>
+          <t>('Sen kväll', '19-21')</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>smoker,dog,&gt;18</t>
+          <t>license,dog</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Getargatan 13</t>
+          <t>Rudagatan 51</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>64.72515988986189</t>
+          <t>64.73076905004987</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>21.081590156187488</t>
+          <t>21.062869127380175</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Individ 16</t>
+          <t>Individ 2</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>('Tidig kväll', '17-19')</t>
+          <t>('Sen kväll', '19-21')</t>
         </is>
       </c>
       <c r="D41" t="inlineStr"/>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Johansgatan 27</t>
+          <t>Rudagatan 41</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>64.72402676388035</t>
+          <t>64.73109609499264</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>21.080091374591447</t>
+          <t>21.065514656793624</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Individ 28</t>
+          <t>Individ 6</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>('Tidig kväll', '17-19')</t>
-        </is>
-      </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>license,cat</t>
-        </is>
-      </c>
+          <t>('Sen kväll', '19-21')</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr"/>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Lillgatan 7A</t>
+          <t>Rudagatan 18</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>64.71565457756343</t>
+          <t>64.72822387894983</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>21.0969892402338</t>
+          <t>21.066092511399347</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Individ 36</t>
+          <t>Individ 6</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -1828,127 +1816,131 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>('Tidig kväll', '17-19')</t>
+          <t>('Sen kväll', '19-21')</t>
         </is>
       </c>
       <c r="D43" t="inlineStr"/>
       <c r="E43" t="inlineStr">
         <is>
-          <t>SkelleftehamnsvÃ¤gen 80</t>
+          <t>Rudagatan 18</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>64.7163138775638</t>
+          <t>64.72822387894983</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>21.15327989790421</t>
+          <t>21.066092511399347</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Individ 53</t>
+          <t>Individ 8</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>('Tidig kväll', '17-19')</t>
+          <t>('Sen kväll', '19-21')</t>
         </is>
       </c>
       <c r="D44" t="inlineStr"/>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Redargatan 11</t>
+          <t>FalmyrvÃ¤gen 58</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>64.70674759364812</t>
+          <t>64.72731282540025</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>21.18053518256285</t>
+          <t>21.07195383043295</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Individ 54</t>
+          <t>Individ 13</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>('Tidig kväll', '17-19')</t>
-        </is>
-      </c>
-      <c r="D45" t="inlineStr"/>
+          <t>('Sen kväll', '19-21')</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>license,&gt;18</t>
+        </is>
+      </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Redargatan 14</t>
+          <t>DiktorpsvÃ¤gen 14</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>64.70605796158435</t>
+          <t>64.72742231880282</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>21.180770669068398</t>
+          <t>21.07853091139931</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Individ 57</t>
+          <t>Individ 14</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>('Tidig kväll', '17-19')</t>
+          <t>('Sen kväll', '19-21')</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>license</t>
+          <t>dog</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Ã–rlogsgatan 28</t>
+          <t>TrÃ¶skargatan 12</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>64.70277797755517</t>
+          <t>64.72569273438936</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>21.18806254023302</t>
+          <t>21.08245052745085</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Individ 60</t>
+          <t>Individ 15</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -1956,131 +1948,135 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>('Tidig kväll', '17-19')</t>
+          <t>('Sen kväll', '19-21')</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>license</t>
+          <t>smoker,dog,&gt;18</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>AlderholmsvÃ¤gen 30</t>
+          <t>Getargatan 13</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>64.6949387916413</t>
+          <t>64.72515988986189</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>21.189652311397285</t>
+          <t>21.081590156187488</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Individ 61</t>
+          <t>Individ 18</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>('Tidig kväll', '17-19')</t>
+          <t>('Sen kväll', '19-21')</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>license</t>
+          <t>license,&gt;18</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>SkelleftehamnsvÃ¤gen 205</t>
+          <t>OmvÃ¤gen 11</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>64.6956845633339</t>
+          <t>64.722700477568</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>21.198373724891763</t>
+          <t>21.076038097904636</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Individ 62</t>
+          <t>Individ 19</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>('Tidig kväll', '17-19')</t>
+          <t>('Sen kväll', '19-21')</t>
         </is>
       </c>
       <c r="D49" t="inlineStr"/>
       <c r="E49" t="inlineStr">
         <is>
-          <t>VÃ¥gens grÃ¤nd 2</t>
+          <t>Holmgatan 22</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>64.69386766364026</t>
+          <t>64.72178804029595</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>21.195669282562054</t>
+          <t>21.078316140234115</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Individ 65</t>
+          <t>Individ 20</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>('Tidig kväll', '17-19')</t>
-        </is>
-      </c>
-      <c r="D50" t="inlineStr"/>
+          <t>('Sen kväll', '19-21')</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>cat</t>
+        </is>
+      </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>HARRBÃ„CKSSAND 152</t>
+          <t>BergsbyvÃ¤gen 19</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>64.72430178226789</t>
+          <t>64.72253627756791</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>21.227400740234213</t>
+          <t>21.081495540234208</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Individ 67</t>
+          <t>Individ 21</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -2088,100 +2084,104 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>('Tidig kväll', '17-19')</t>
-        </is>
-      </c>
-      <c r="D51" t="inlineStr"/>
+          <t>('Sen kväll', '19-21')</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>&gt;18</t>
+        </is>
+      </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Styrmansgatan 9</t>
+          <t>Nybyggargatan 12</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>64.70799259606436</t>
+          <t>64.72279765876095</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>21.178082469068517</t>
+          <t>21.096477997904646</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Individ 69</t>
+          <t>Individ 22</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>('Tidig kväll', '17-19')</t>
-        </is>
-      </c>
-      <c r="D52" t="inlineStr"/>
+          <t>('Sen kväll', '19-21')</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>dog</t>
+        </is>
+      </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>BokgrÃ¤nd 7</t>
+          <t>Nybyggargatan 13</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>64.71491237756301</t>
+          <t>64.7221138654314</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>21.158029382563345</t>
+          <t>21.096186911398974</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Individ 1</t>
+          <t>Individ 23</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
           <t>('Sen kväll', '19-21')</t>
         </is>
       </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>license,dog</t>
-        </is>
-      </c>
+      <c r="D53" t="inlineStr"/>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Rudagatan 51</t>
+          <t>Nybyggargatan 6B</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>64.73076905004987</t>
+          <t>64.71991329588566</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>21.062869127380175</t>
+          <t>21.094155711398862</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Individ 2</t>
+          <t>Individ 24</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
@@ -2191,28 +2191,28 @@
       <c r="D54" t="inlineStr"/>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Rudagatan 41</t>
+          <t>Roddargatan 12</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>64.73109609499264</t>
+          <t>64.71749269547423</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>21.065514656793624</t>
+          <t>21.09246261139871</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Individ 6</t>
+          <t>Individ 26</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
@@ -2222,86 +2222,94 @@
       <c r="D55" t="inlineStr"/>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Rudagatan 18</t>
+          <t>Roddargatan 17</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>64.72822387894983</t>
+          <t>64.7169136063257</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>21.066092511399347</t>
+          <t>21.09606822673948</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Individ 6</t>
+          <t>Individ 27</t>
         </is>
       </c>
       <c r="B56" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
           <t>('Sen kväll', '19-21')</t>
         </is>
       </c>
-      <c r="D56" t="inlineStr"/>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>smoker,&gt;18</t>
+        </is>
+      </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>Rudagatan 18</t>
+          <t>Lillgatan 4</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>64.72822387894983</t>
+          <t>64.71611465988815</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>21.066092511399347</t>
+          <t>21.09484154023385</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Individ 8</t>
+          <t>Individ 39</t>
         </is>
       </c>
       <c r="B57" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
           <t>('Sen kväll', '19-21')</t>
         </is>
       </c>
-      <c r="D57" t="inlineStr"/>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>smoker</t>
+        </is>
+      </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>FalmyrvÃ¤gen 58</t>
+          <t>MÃ¥bÃ¤rsgatan 9</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>64.72731282540025</t>
+          <t>64.71710435972129</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>21.07195383043295</t>
+          <t>21.156185624893038</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Individ 13</t>
+          <t>Individ 40</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -2314,33 +2322,33 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>license,&gt;18</t>
+          <t>license</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>DiktorpsvÃ¤gen 14</t>
+          <t>Karagangatan 7</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>64.72742231880282</t>
+          <t>64.71669937756415</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>21.07853091139931</t>
+          <t>21.16159071139863</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Individ 14</t>
+          <t>Individ 40</t>
         </is>
       </c>
       <c r="B59" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
@@ -2349,29 +2357,29 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>dog</t>
+          <t>license</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>TrÃ¶skargatan 12</t>
+          <t>Karagangatan 7</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>64.72569273438936</t>
+          <t>64.71669937756415</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>21.08245052745085</t>
+          <t>21.16159071139863</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Individ 15</t>
+          <t>Individ 41</t>
         </is>
       </c>
       <c r="B60" t="n">
@@ -2384,68 +2392,64 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>smoker,dog,&gt;18</t>
+          <t>license</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>Getargatan 13</t>
+          <t>SkelleftehamnsvÃ¤gen 113</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>64.72515988986189</t>
+          <t>64.7145646253258</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>21.081590156187488</t>
+          <t>21.16073439790411</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Individ 18</t>
+          <t>Individ 47</t>
         </is>
       </c>
       <c r="B61" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
           <t>('Sen kväll', '19-21')</t>
         </is>
       </c>
-      <c r="D61" t="inlineStr">
-        <is>
-          <t>license,&gt;18</t>
-        </is>
-      </c>
+      <c r="D61" t="inlineStr"/>
       <c r="E61" t="inlineStr">
         <is>
-          <t>OmvÃ¤gen 11</t>
+          <t>SandgÃ¤rdsvÃ¤gen 33</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>64.722700477568</t>
+          <t>64.71030057755999</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>21.076038097904636</t>
+          <t>21.18197034023344</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Individ 19</t>
+          <t>Individ 50</t>
         </is>
       </c>
       <c r="B62" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
@@ -2455,133 +2459,121 @@
       <c r="D62" t="inlineStr"/>
       <c r="E62" t="inlineStr">
         <is>
-          <t>Holmgatan 22</t>
+          <t>BrÃ¶drahemsgatan 16</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>64.72178804029595</t>
+          <t>64.71090737756037</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>21.078316140234115</t>
+          <t>21.17480491139828</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Individ 20</t>
+          <t>Individ 51</t>
         </is>
       </c>
       <c r="B63" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
           <t>('Sen kväll', '19-21')</t>
         </is>
       </c>
-      <c r="D63" t="inlineStr">
-        <is>
-          <t>cat</t>
-        </is>
-      </c>
+      <c r="D63" t="inlineStr"/>
       <c r="E63" t="inlineStr">
         <is>
-          <t>BergsbyvÃ¤gen 19</t>
+          <t>SkyttevÃ¤gen 3</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>64.72253627756791</t>
+          <t>64.70942679485121</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>21.081495540234208</t>
+          <t>21.17345478256298</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Individ 21</t>
+          <t>Individ 59</t>
         </is>
       </c>
       <c r="B64" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C64" t="inlineStr">
         <is>
           <t>('Sen kväll', '19-21')</t>
         </is>
       </c>
-      <c r="D64" t="inlineStr">
-        <is>
-          <t>&gt;18</t>
-        </is>
-      </c>
+      <c r="D64" t="inlineStr"/>
       <c r="E64" t="inlineStr">
         <is>
-          <t>Nybyggargatan 12</t>
+          <t>Lotsens grÃ¤nd 5</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>64.72279765876095</t>
+          <t>64.69594034903153</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>21.096477997904646</t>
+          <t>21.190897069067788</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Individ 22</t>
+          <t>Individ 63</t>
         </is>
       </c>
       <c r="B65" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
           <t>('Sen kväll', '19-21')</t>
         </is>
       </c>
-      <c r="D65" t="inlineStr">
-        <is>
-          <t>dog</t>
-        </is>
-      </c>
+      <c r="D65" t="inlineStr"/>
       <c r="E65" t="inlineStr">
         <is>
-          <t>Nybyggargatan 13</t>
+          <t>SÃ¶dra Sillskatan 510</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>64.7221138654314</t>
+          <t>64.72975809755901</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>21.096186911398974</t>
+          <t>21.220638097905063</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Individ 23</t>
+          <t>Individ 70</t>
         </is>
       </c>
       <c r="B66" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
@@ -2591,615 +2583,17 @@
       <c r="D66" t="inlineStr"/>
       <c r="E66" t="inlineStr">
         <is>
-          <t>Nybyggargatan 6B</t>
+          <t>Hagtornsgatan 39</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>64.71991329588566</t>
+          <t>64.719327050046</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>21.094155711398862</t>
-        </is>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="inlineStr">
-        <is>
-          <t>Individ 24</t>
-        </is>
-      </c>
-      <c r="B67" t="n">
-        <v>10</v>
-      </c>
-      <c r="C67" t="inlineStr">
-        <is>
-          <t>('Sen kväll', '19-21')</t>
-        </is>
-      </c>
-      <c r="D67" t="inlineStr"/>
-      <c r="E67" t="inlineStr">
-        <is>
-          <t>Roddargatan 12</t>
-        </is>
-      </c>
-      <c r="F67" t="inlineStr">
-        <is>
-          <t>64.71749269547423</t>
-        </is>
-      </c>
-      <c r="G67" t="inlineStr">
-        <is>
-          <t>21.09246261139871</t>
-        </is>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="inlineStr">
-        <is>
-          <t>Individ 26</t>
-        </is>
-      </c>
-      <c r="B68" t="n">
-        <v>10</v>
-      </c>
-      <c r="C68" t="inlineStr">
-        <is>
-          <t>('Sen kväll', '19-21')</t>
-        </is>
-      </c>
-      <c r="D68" t="inlineStr"/>
-      <c r="E68" t="inlineStr">
-        <is>
-          <t>Roddargatan 17</t>
-        </is>
-      </c>
-      <c r="F68" t="inlineStr">
-        <is>
-          <t>64.7169136063257</t>
-        </is>
-      </c>
-      <c r="G68" t="inlineStr">
-        <is>
-          <t>21.09606822673948</t>
-        </is>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>Individ 27</t>
-        </is>
-      </c>
-      <c r="B69" t="n">
-        <v>10</v>
-      </c>
-      <c r="C69" t="inlineStr">
-        <is>
-          <t>('Sen kväll', '19-21')</t>
-        </is>
-      </c>
-      <c r="D69" t="inlineStr">
-        <is>
-          <t>smoker,&gt;18</t>
-        </is>
-      </c>
-      <c r="E69" t="inlineStr">
-        <is>
-          <t>Lillgatan 4</t>
-        </is>
-      </c>
-      <c r="F69" t="inlineStr">
-        <is>
-          <t>64.71611465988815</t>
-        </is>
-      </c>
-      <c r="G69" t="inlineStr">
-        <is>
-          <t>21.09484154023385</t>
-        </is>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="inlineStr">
-        <is>
-          <t>Individ 39</t>
-        </is>
-      </c>
-      <c r="B70" t="n">
-        <v>5</v>
-      </c>
-      <c r="C70" t="inlineStr">
-        <is>
-          <t>('Sen kväll', '19-21')</t>
-        </is>
-      </c>
-      <c r="D70" t="inlineStr">
-        <is>
-          <t>smoker</t>
-        </is>
-      </c>
-      <c r="E70" t="inlineStr">
-        <is>
-          <t>MÃ¥bÃ¤rsgatan 9</t>
-        </is>
-      </c>
-      <c r="F70" t="inlineStr">
-        <is>
-          <t>64.71710435972129</t>
-        </is>
-      </c>
-      <c r="G70" t="inlineStr">
-        <is>
-          <t>21.156185624893038</t>
-        </is>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="inlineStr">
-        <is>
-          <t>Individ 40</t>
-        </is>
-      </c>
-      <c r="B71" t="n">
-        <v>15</v>
-      </c>
-      <c r="C71" t="inlineStr">
-        <is>
-          <t>('Sen kväll', '19-21')</t>
-        </is>
-      </c>
-      <c r="D71" t="inlineStr">
-        <is>
-          <t>license</t>
-        </is>
-      </c>
-      <c r="E71" t="inlineStr">
-        <is>
-          <t>Karagangatan 7</t>
-        </is>
-      </c>
-      <c r="F71" t="inlineStr">
-        <is>
-          <t>64.71669937756415</t>
-        </is>
-      </c>
-      <c r="G71" t="inlineStr">
-        <is>
-          <t>21.16159071139863</t>
-        </is>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>Individ 40</t>
-        </is>
-      </c>
-      <c r="B72" t="n">
-        <v>15</v>
-      </c>
-      <c r="C72" t="inlineStr">
-        <is>
-          <t>('Sen kväll', '19-21')</t>
-        </is>
-      </c>
-      <c r="D72" t="inlineStr">
-        <is>
-          <t>license</t>
-        </is>
-      </c>
-      <c r="E72" t="inlineStr">
-        <is>
-          <t>Karagangatan 7</t>
-        </is>
-      </c>
-      <c r="F72" t="inlineStr">
-        <is>
-          <t>64.71669937756415</t>
-        </is>
-      </c>
-      <c r="G72" t="inlineStr">
-        <is>
-          <t>21.16159071139863</t>
-        </is>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="inlineStr">
-        <is>
-          <t>Individ 41</t>
-        </is>
-      </c>
-      <c r="B73" t="n">
-        <v>10</v>
-      </c>
-      <c r="C73" t="inlineStr">
-        <is>
-          <t>('Sen kväll', '19-21')</t>
-        </is>
-      </c>
-      <c r="D73" t="inlineStr">
-        <is>
-          <t>license</t>
-        </is>
-      </c>
-      <c r="E73" t="inlineStr">
-        <is>
-          <t>SkelleftehamnsvÃ¤gen 113</t>
-        </is>
-      </c>
-      <c r="F73" t="inlineStr">
-        <is>
-          <t>64.7145646253258</t>
-        </is>
-      </c>
-      <c r="G73" t="inlineStr">
-        <is>
-          <t>21.16073439790411</t>
-        </is>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="inlineStr">
-        <is>
-          <t>Individ 47</t>
-        </is>
-      </c>
-      <c r="B74" t="n">
-        <v>5</v>
-      </c>
-      <c r="C74" t="inlineStr">
-        <is>
-          <t>('Sen kväll', '19-21')</t>
-        </is>
-      </c>
-      <c r="D74" t="inlineStr"/>
-      <c r="E74" t="inlineStr">
-        <is>
-          <t>SandgÃ¤rdsvÃ¤gen 33</t>
-        </is>
-      </c>
-      <c r="F74" t="inlineStr">
-        <is>
-          <t>64.71030057755999</t>
-        </is>
-      </c>
-      <c r="G74" t="inlineStr">
-        <is>
-          <t>21.18197034023344</t>
-        </is>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="inlineStr">
-        <is>
-          <t>Individ 50</t>
-        </is>
-      </c>
-      <c r="B75" t="n">
-        <v>10</v>
-      </c>
-      <c r="C75" t="inlineStr">
-        <is>
-          <t>('Sen kväll', '19-21')</t>
-        </is>
-      </c>
-      <c r="D75" t="inlineStr"/>
-      <c r="E75" t="inlineStr">
-        <is>
-          <t>BrÃ¶drahemsgatan 16</t>
-        </is>
-      </c>
-      <c r="F75" t="inlineStr">
-        <is>
-          <t>64.71090737756037</t>
-        </is>
-      </c>
-      <c r="G75" t="inlineStr">
-        <is>
-          <t>21.17480491139828</t>
-        </is>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="inlineStr">
-        <is>
-          <t>Individ 51</t>
-        </is>
-      </c>
-      <c r="B76" t="n">
-        <v>15</v>
-      </c>
-      <c r="C76" t="inlineStr">
-        <is>
-          <t>('Sen kväll', '19-21')</t>
-        </is>
-      </c>
-      <c r="D76" t="inlineStr"/>
-      <c r="E76" t="inlineStr">
-        <is>
-          <t>SkyttevÃ¤gen 3</t>
-        </is>
-      </c>
-      <c r="F76" t="inlineStr">
-        <is>
-          <t>64.70942679485121</t>
-        </is>
-      </c>
-      <c r="G76" t="inlineStr">
-        <is>
-          <t>21.17345478256298</t>
-        </is>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="inlineStr">
-        <is>
-          <t>Individ 59</t>
-        </is>
-      </c>
-      <c r="B77" t="n">
-        <v>15</v>
-      </c>
-      <c r="C77" t="inlineStr">
-        <is>
-          <t>('Sen kväll', '19-21')</t>
-        </is>
-      </c>
-      <c r="D77" t="inlineStr"/>
-      <c r="E77" t="inlineStr">
-        <is>
-          <t>Lotsens grÃ¤nd 5</t>
-        </is>
-      </c>
-      <c r="F77" t="inlineStr">
-        <is>
-          <t>64.69594034903153</t>
-        </is>
-      </c>
-      <c r="G77" t="inlineStr">
-        <is>
-          <t>21.190897069067788</t>
-        </is>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="inlineStr">
-        <is>
-          <t>Individ 63</t>
-        </is>
-      </c>
-      <c r="B78" t="n">
-        <v>7</v>
-      </c>
-      <c r="C78" t="inlineStr">
-        <is>
-          <t>('Sen kväll', '19-21')</t>
-        </is>
-      </c>
-      <c r="D78" t="inlineStr"/>
-      <c r="E78" t="inlineStr">
-        <is>
-          <t>SÃ¶dra Sillskatan 510</t>
-        </is>
-      </c>
-      <c r="F78" t="inlineStr">
-        <is>
-          <t>64.72975809755901</t>
-        </is>
-      </c>
-      <c r="G78" t="inlineStr">
-        <is>
-          <t>21.220638097905063</t>
-        </is>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="inlineStr">
-        <is>
-          <t>Individ 70</t>
-        </is>
-      </c>
-      <c r="B79" t="n">
-        <v>10</v>
-      </c>
-      <c r="C79" t="inlineStr">
-        <is>
-          <t>('Sen kväll', '19-21')</t>
-        </is>
-      </c>
-      <c r="D79" t="inlineStr"/>
-      <c r="E79" t="inlineStr">
-        <is>
-          <t>Hagtornsgatan 39</t>
-        </is>
-      </c>
-      <c r="F79" t="inlineStr">
-        <is>
-          <t>64.719327050046</t>
-        </is>
-      </c>
-      <c r="G79" t="inlineStr">
-        <is>
           <t>21.15099431139883</t>
-        </is>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="inlineStr">
-        <is>
-          <t>Individ 1</t>
-        </is>
-      </c>
-      <c r="B80" t="n">
-        <v>30</v>
-      </c>
-      <c r="C80" t="inlineStr">
-        <is>
-          <t>('Förmiddag', '9-11')</t>
-        </is>
-      </c>
-      <c r="D80" t="inlineStr">
-        <is>
-          <t>license,dog,woman</t>
-        </is>
-      </c>
-      <c r="E80" t="inlineStr">
-        <is>
-          <t>Rudagatan 51</t>
-        </is>
-      </c>
-      <c r="F80" t="inlineStr">
-        <is>
-          <t>64.73076905004987</t>
-        </is>
-      </c>
-      <c r="G80" t="inlineStr">
-        <is>
-          <t>21.062869127380175</t>
-        </is>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="inlineStr">
-        <is>
-          <t>Individ 28</t>
-        </is>
-      </c>
-      <c r="B81" t="n">
-        <v>20</v>
-      </c>
-      <c r="C81" t="inlineStr">
-        <is>
-          <t>('Förmiddag', '9-11')</t>
-        </is>
-      </c>
-      <c r="D81" t="inlineStr">
-        <is>
-          <t>license,cat</t>
-        </is>
-      </c>
-      <c r="E81" t="inlineStr">
-        <is>
-          <t>Lillgatan 7A</t>
-        </is>
-      </c>
-      <c r="F81" t="inlineStr">
-        <is>
-          <t>64.71565457756343</t>
-        </is>
-      </c>
-      <c r="G81" t="inlineStr">
-        <is>
-          <t>21.0969892402338</t>
-        </is>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="inlineStr">
-        <is>
-          <t>Individ 29</t>
-        </is>
-      </c>
-      <c r="B82" t="n">
-        <v>40</v>
-      </c>
-      <c r="C82" t="inlineStr">
-        <is>
-          <t>('Förmiddag', '9-11')</t>
-        </is>
-      </c>
-      <c r="D82" t="inlineStr">
-        <is>
-          <t>license</t>
-        </is>
-      </c>
-      <c r="E82" t="inlineStr">
-        <is>
-          <t>Roddargatan 29</t>
-        </is>
-      </c>
-      <c r="F82" t="inlineStr">
-        <is>
-          <t>64.7158097128137</t>
-        </is>
-      </c>
-      <c r="G82" t="inlineStr">
-        <is>
-          <t>21.098717311398616</t>
-        </is>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="inlineStr">
-        <is>
-          <t>Individ 37</t>
-        </is>
-      </c>
-      <c r="B83" t="n">
-        <v>20</v>
-      </c>
-      <c r="C83" t="inlineStr">
-        <is>
-          <t>('Eftermiddag', '13-15')</t>
-        </is>
-      </c>
-      <c r="D83" t="inlineStr">
-        <is>
-          <t>license</t>
-        </is>
-      </c>
-      <c r="E83" t="inlineStr">
-        <is>
-          <t>MÃ¥bÃ¤rsgatan 12</t>
-        </is>
-      </c>
-      <c r="F83" t="inlineStr">
-        <is>
-          <t>64.71651135982128</t>
-        </is>
-      </c>
-      <c r="G83" t="inlineStr">
-        <is>
-          <t>21.15559144023381</t>
-        </is>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="inlineStr">
-        <is>
-          <t>Individ 38</t>
-        </is>
-      </c>
-      <c r="B84" t="n">
-        <v>45</v>
-      </c>
-      <c r="C84" t="inlineStr">
-        <is>
-          <t>('Eftermiddag', '13-15')</t>
-        </is>
-      </c>
-      <c r="D84" t="inlineStr">
-        <is>
-          <t>license</t>
-        </is>
-      </c>
-      <c r="E84" t="inlineStr">
-        <is>
-          <t>Karagangatan 30</t>
-        </is>
-      </c>
-      <c r="F84" t="inlineStr">
-        <is>
-          <t>64.71678347084324</t>
-        </is>
-      </c>
-      <c r="G84" t="inlineStr">
-        <is>
-          <t>21.15778882489306</t>
         </is>
       </c>
     </row>

</xml_diff>